<commit_message>
Code modified, Now same contact can get multiple messages.
</commit_message>
<xml_diff>
--- a/project/contacts.xlsx
+++ b/project/contacts.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>Name</t>
   </si>
@@ -27,10 +27,7 @@
     <t>Phone</t>
   </si>
   <si>
-    <t>Ashraful Hussain Khan</t>
-  </si>
-  <si>
-    <t>Hafiz</t>
+    <t>Ashraful</t>
   </si>
 </sst>
 </file>
@@ -348,10 +345,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -376,14 +373,6 @@
         <v>917406113544</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3">
-        <v>917406966472</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>